<commit_message>
feat: adicionar botão de voltar ao dashboard em Upload e Mapas e correções
</commit_message>
<xml_diff>
--- a/backend/output/915198_V0.1.xlsx
+++ b/backend/output/915198_V0.1.xlsx
@@ -2317,7 +2317,7 @@
       <c r="I32" s="7" t="inlineStr"/>
       <c r="J32" s="12" t="inlineStr">
         <is>
-          <t>22/05/2025</t>
+          <t>26/05/2025</t>
         </is>
       </c>
       <c r="K32" s="37" t="n"/>
@@ -3583,7 +3583,7 @@
       <c r="G31" s="7" t="inlineStr"/>
       <c r="H31" s="12" t="inlineStr">
         <is>
-          <t>22/05/2025</t>
+          <t>26/05/2025</t>
         </is>
       </c>
       <c r="J31" s="37" t="n"/>

</xml_diff>